<commit_message>
Data updates removing extra peak timeslice
</commit_message>
<xml_diff>
--- a/InputData/elec/LFHVM/Load Factor Hourly Variance Multiplier.xlsx
+++ b/InputData/elec/LFHVM/Load Factor Hourly Variance Multiplier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\LFHVM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\LFHVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB1ADFA-1C6C-49EE-B51F-B05B98A7EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB475A61-37DD-4079-87FF-63CDE72F6CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="3060" windowWidth="19710" windowHeight="20325" xr2:uid="{E755D2B6-154D-4132-AE62-7719D42AA9EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{E755D2B6-154D-4132-AE62-7719D42AA9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>LFHVM Load Factor Hourly Variance Multiplier</t>
   </si>
@@ -96,36 +96,6 @@
     <t>Fall</t>
   </si>
   <si>
-    <t>Summer Peak 1</t>
-  </si>
-  <si>
-    <t>Summer Peak 2</t>
-  </si>
-  <si>
-    <t>Summer Peak 3</t>
-  </si>
-  <si>
-    <t>Summer Peak 4</t>
-  </si>
-  <si>
-    <t>Summer Peak 5</t>
-  </si>
-  <si>
-    <t>Winter Peak 1</t>
-  </si>
-  <si>
-    <t>Winter Peak 2</t>
-  </si>
-  <si>
-    <t>Winter Peak 3</t>
-  </si>
-  <si>
-    <t>Winter Peak 4</t>
-  </si>
-  <si>
-    <t>Winter Peak 5</t>
-  </si>
-  <si>
     <t>transportation sector</t>
   </si>
   <si>
@@ -151,6 +121,12 @@
   </si>
   <si>
     <t>Units: dimensionless</t>
+  </si>
+  <si>
+    <t>Summer Peak</t>
+  </si>
+  <si>
+    <t>Winter Peak</t>
   </si>
 </sst>
 </file>
@@ -648,9 +624,11 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -660,31 +638,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -805,7 +783,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6">
         <v>0.64</v>
@@ -834,7 +812,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6">
         <v>0.64</v>
@@ -858,238 +836,6 @@
         <v>0.64</v>
       </c>
       <c r="I7" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="I15" s="6">
         <v>0.64</v>
       </c>
     </row>

</xml_diff>